<commit_message>
ConsolidateData, Update Stage -> NDS
</commit_message>
<xml_diff>
--- a/Ontario_Covid/Report/NDS/ConsolidateData.xlsx
+++ b/Ontario_Covid/Report/NDS/ConsolidateData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\University\4th-year\HKI\BI\Thực hành\Project\Ontario_Covid\Ontario_Covid\Report\NDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F4335A-9FE5-45D3-9E39-073D2F6B38E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF4BE65-5A88-4B81-92B2-71F6968871A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,18 +225,6 @@
     <t>Not Reported - Không được báo cáo</t>
   </si>
   <si>
-    <t>Outbreak → OB</t>
-  </si>
-  <si>
-    <t>Close Contact → CC</t>
-  </si>
-  <si>
-    <t>Travel-Related → Travel</t>
-  </si>
-  <si>
-    <t>Not Reported → No known Epi-link</t>
-  </si>
-  <si>
     <t>NDS</t>
   </si>
   <si>
@@ -343,6 +331,18 @@
   </si>
   <si>
     <t>Agegroup → Age_Group</t>
+  </si>
+  <si>
+    <t>OB → Outbreak</t>
+  </si>
+  <si>
+    <t>CC → Close Contact</t>
+  </si>
+  <si>
+    <t>No known Epi-link → Not Reported</t>
+  </si>
+  <si>
+    <t>Travel → Travel-Related</t>
   </si>
 </sst>
 </file>
@@ -621,13 +621,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -636,12 +642,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -651,13 +651,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,25 +669,28 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -699,13 +702,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A47"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,10 +1015,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="34"/>
-      <c r="E1" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="23"/>
+      <c r="E1" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -1034,10 +1034,10 @@
         <v>12</v>
       </c>
       <c r="E2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>79</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1050,8 +1050,8 @@
         <v>13</v>
       </c>
       <c r="E3" s="27"/>
-      <c r="F3" s="38" t="s">
-        <v>88</v>
+      <c r="F3" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1062,8 +1062,8 @@
         <v>11</v>
       </c>
       <c r="E4" s="27"/>
-      <c r="F4" s="38" t="s">
-        <v>81</v>
+      <c r="F4" s="19" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1080,8 +1080,8 @@
         <v>35</v>
       </c>
       <c r="E5" s="27"/>
-      <c r="F5" s="38" t="s">
-        <v>84</v>
+      <c r="F5" s="19" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1094,8 +1094,8 @@
         <v>28</v>
       </c>
       <c r="E6" s="27"/>
-      <c r="F6" s="38" t="s">
-        <v>80</v>
+      <c r="F6" s="19" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1108,8 +1108,8 @@
         <v>29</v>
       </c>
       <c r="E7" s="27"/>
-      <c r="F7" s="38" t="s">
-        <v>86</v>
+      <c r="F7" s="19" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1122,8 +1122,8 @@
         <v>30</v>
       </c>
       <c r="E8" s="27"/>
-      <c r="F8" s="38" t="s">
-        <v>91</v>
+      <c r="F8" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1136,8 +1136,8 @@
         <v>31</v>
       </c>
       <c r="E9" s="27"/>
-      <c r="F9" s="38" t="s">
-        <v>89</v>
+      <c r="F9" s="19" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1150,8 +1150,8 @@
         <v>32</v>
       </c>
       <c r="E10" s="27"/>
-      <c r="F10" s="38" t="s">
-        <v>87</v>
+      <c r="F10" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1164,8 +1164,8 @@
         <v>33</v>
       </c>
       <c r="E11" s="27"/>
-      <c r="F11" s="38" t="s">
-        <v>90</v>
+      <c r="F11" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1178,8 +1178,8 @@
         <v>34</v>
       </c>
       <c r="E12" s="27"/>
-      <c r="F12" s="38" t="s">
-        <v>85</v>
+      <c r="F12" s="19" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1192,7 +1192,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="27"/>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1210,8 +1210,8 @@
         <v>24</v>
       </c>
       <c r="E14" s="28"/>
-      <c r="F14" s="38" t="s">
-        <v>82</v>
+      <c r="F14" s="19" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -1225,13 +1225,13 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="29" t="s">
         <v>57</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -1239,54 +1239,54 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="37"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="23"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="25"/>
     </row>
     <row r="23" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>71</v>
+      <c r="C23" s="40" t="s">
+        <v>67</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>12</v>
@@ -1297,7 +1297,7 @@
       <c r="B24" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="11" t="s">
         <v>13</v>
       </c>
@@ -1305,219 +1305,219 @@
     <row r="25" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="28"/>
       <c r="B25" s="17"/>
-      <c r="C25" s="21"/>
+      <c r="C25" s="41"/>
       <c r="D25" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
-        <v>73</v>
+      <c r="A26" s="37" t="s">
+        <v>69</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="45" t="s">
+      <c r="C26" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="47" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="30"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="46"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="30"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="46" t="s">
+      <c r="C28" s="44"/>
+      <c r="D28" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="30"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="46"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="23"/>
     </row>
     <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="30"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="46" t="s">
+      <c r="C30" s="44"/>
+      <c r="D30" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="46"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="23"/>
     </row>
     <row r="32" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="30"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="46" t="s">
+      <c r="C32" s="44"/>
+      <c r="D32" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="30"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="46"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="23"/>
     </row>
     <row r="34" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="31"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="46" t="s">
+      <c r="C34" s="44"/>
+      <c r="D34" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="46"/>
+        <v>101</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="44"/>
+      <c r="D35" s="23"/>
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
-      <c r="B36" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="46" t="s">
+      <c r="B36" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="44"/>
+      <c r="D36" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="27"/>
-      <c r="B37" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="46"/>
+      <c r="B37" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="44"/>
+      <c r="D37" s="23"/>
     </row>
     <row r="38" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="27"/>
-      <c r="B38" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="46" t="s">
+      <c r="B38" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="44"/>
+      <c r="D38" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
-      <c r="B39" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="46"/>
+      <c r="B39" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="44"/>
+      <c r="D39" s="23"/>
     </row>
     <row r="40" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="27"/>
-      <c r="B40" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="46" t="s">
+      <c r="B40" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="44"/>
+      <c r="D40" s="23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="27"/>
-      <c r="B41" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="46"/>
+      <c r="B41" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="44"/>
+      <c r="D41" s="23"/>
     </row>
     <row r="42" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="27"/>
-      <c r="B42" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="43"/>
-      <c r="D42" s="46" t="s">
+      <c r="B42" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="44"/>
+      <c r="D42" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="27"/>
-      <c r="B43" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="46"/>
+      <c r="B43" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="44"/>
+      <c r="D43" s="23"/>
     </row>
     <row r="44" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="27"/>
-      <c r="B44" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="46"/>
+      <c r="B44" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="44"/>
+      <c r="D44" s="23"/>
     </row>
     <row r="45" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" s="27"/>
-      <c r="B45" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="46"/>
+      <c r="B45" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="44"/>
+      <c r="D45" s="23"/>
     </row>
     <row r="46" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="27"/>
-      <c r="B46" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="46"/>
+      <c r="B46" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="44"/>
+      <c r="D46" s="23"/>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="28"/>
-      <c r="B47" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="47"/>
+      <c r="B47" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="45"/>
+      <c r="D47" s="46"/>
     </row>
     <row r="48" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A48" s="19" t="s">
-        <v>74</v>
+      <c r="A48" s="40" t="s">
+        <v>70</v>
       </c>
       <c r="B48" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="40" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="5" t="s">
@@ -1525,61 +1525,79 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A49" s="21"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="21"/>
+      <c r="C49" s="41"/>
       <c r="D49" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="s">
-        <v>75</v>
+      <c r="A50" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>77</v>
+        <v>102</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>73</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="30"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="20"/>
+        <v>103</v>
+      </c>
+      <c r="C51" s="42"/>
       <c r="D51" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="30"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="20"/>
+        <v>104</v>
+      </c>
+      <c r="C52" s="42"/>
       <c r="D52" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="31"/>
+      <c r="A53" s="39"/>
       <c r="B53" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="21"/>
+        <v>105</v>
+      </c>
+      <c r="C53" s="41"/>
       <c r="D53" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C26:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A35:A47"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C50:C53"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="E2:E14"/>
@@ -1596,24 +1614,6 @@
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A34"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A35:A47"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C26:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>